<commit_message>
atualizacao post empresas com nova base
</commit_message>
<xml_diff>
--- a/_posts/2020-10-23-empresas/cvm_empresas_problemas.xlsx
+++ b/_posts/2020-10-23-empresas/cvm_empresas_problemas.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -681,319 +681,419 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>1456</v>
+        <v>900</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>47.894.290/0001-28</t>
+          <t>71.473.820/0012-12</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>PLANIN AUDITORES INDEPENDENTES  S/C</t>
+          <t>MILLENNIUM CCVM S/A, SUCESSORA DA GAMEX SECURITIES CCVM LTDA.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2001&amp;NumProc=8739</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=2002&amp;NumProc=15</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>397</v>
+        <v>1456</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>09.143.363/0001-50</t>
+          <t>47.894.290/0001-28</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>EASE ESCRITÓRIO DE AUDITORIA INDEPENDENTE S/C</t>
+          <t>PLANIN AUDITORES INDEPENDENTES  S/C</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2013&amp;NumProc=13481</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2001&amp;NumProc=8739</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>62.030.762/0001-98</t>
+          <t>09.143.363/0001-50</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>AKW AUDITORES INDEPENDENTES S/S</t>
+          <t>EASE ESCRITÓRIO DE AUDITORIA INDEPENDENTE S/C</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2013&amp;NumProc=4362</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2013&amp;NumProc=13481</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>1165</v>
+        <v>411</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>67.634.717/0001-66</t>
+          <t>62.030.762/0001-98</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>BWEL AUDITORES INDEPENDENTES SOCIEDADE SIMPLES</t>
+          <t>AKW AUDITORES INDEPENDENTES S/S</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2017&amp;NumProc=2253</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2013&amp;NumProc=4362</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>427</v>
+        <v>1165</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11.245.719/0003-70</t>
+          <t>67.634.717/0001-66</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>DIRECTA AUDITORES</t>
+          <t>BWEL AUDITORES INDEPENDENTES SOCIEDADE SIMPLES</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2013&amp;NumProc=5682</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2017&amp;NumProc=2253</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>1688</v>
+        <v>427</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>58.214.958/0001-65</t>
+          <t>11.245.719/0003-70</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>SOC TEC AUDITORIA SOMATEC SC</t>
+          <t>DIRECTA AUDITORES</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=2000&amp;NumProc=6</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2013&amp;NumProc=5682</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>844</v>
+        <v>1688</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>31.622.483/0001-90</t>
+          <t>58.214.958/0001-65</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>GUILHERME FONTES FILMES LTDA.</t>
+          <t>SOC TEC AUDITORIA SOMATEC SC</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=2000&amp;NumProc=12</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=2000&amp;NumProc=6</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>52</v>
+        <v>844</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>04.612.682/0001-44</t>
+          <t>31.622.483/0001-90</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>INTERTRADING AGRONEGÓCIOS LTDA.</t>
+          <t>GUILHERME FONTES FILMES LTDA.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2007&amp;NumProc=4414</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=2000&amp;NumProc=12</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>21</v>
+        <v>1035</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>27.901.719/0001-50</t>
+          <t>00.469.585/0001-93</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>INSTITUTO AERUS DE SEGURIDADE SOCIAL</t>
+          <t>FACEB - FUNDAÇÃO DE ASSISTÊNCIA DOS EMPREGADOS DA CEB</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2007&amp;NumProc=1176</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=1999&amp;NumProc=28</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>555</v>
+        <v>1035</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>64.920.416/0001-00</t>
+          <t>17.393.471/0001-13</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>NORMAS AUDITORES INDEPENDENTES</t>
+          <t>PRATA DTVM LTDA. (atual Prata Consultoria e Assessoria Empresarial Ltda.)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2015&amp;NumProc=11941</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=1999&amp;NumProc=28</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>1565</v>
+        <v>52</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>43.729.789/0001-29</t>
+          <t>04.612.682/0001-44</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>PERMALI DO BRASIL INDÚSTRIA E COMÉRCIO LTDA</t>
+          <t>INTERTRADING AGRONEGÓCIOS LTDA.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2005&amp;NumProc=33</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2007&amp;NumProc=4414</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>1556</v>
+        <v>21</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>04.565.230/0002-30</t>
+          <t>27.901.719/0001-50</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>I.B. Sabbá S/A</t>
+          <t>INSTITUTO AERUS DE SEGURIDADE SOCIAL</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2004&amp;NumProc=4627</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2007&amp;NumProc=1176</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>217</v>
+        <v>1563</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>05.723.617/0001-59</t>
+          <t>43.214.485/0001-29</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MAPFRE DTVM S.A.</t>
+          <t>SOCIVAL AUDITORIA INDEP SC</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2010&amp;NumProc=17292</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2004&amp;NumProc=7001</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>642</v>
+        <v>555</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>05.706.592/0001-85</t>
+          <t>64.920.416/0001-00</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>BANCO BOZANO, SIMONSEN S/A</t>
+          <t>NORMAS AUDITORES INDEPENDENTES</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=1999&amp;NumProc=10</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2015&amp;NumProc=11941</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>2</v>
+        <v>1565</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>00.659.559/0002-09</t>
+          <t>43.729.789/0001-29</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MASTER CORRETORA DE MERCADORIAS LTDA.</t>
+          <t>PERMALI DO BRASIL INDÚSTRIA E COMÉRCIO LTDA</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=2006&amp;NumProc=1</t>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2005&amp;NumProc=33</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32">
+        <v>1556</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>04.565.230/0002-30</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>I.B. Sabbá S/A</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2004&amp;NumProc=4627</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>217</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>05.723.617/0001-59</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>MAPFRE DTVM S.A.</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2010&amp;NumProc=17292</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>1710</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14.629.882/0001-63</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>CAPITAL ASSESSORIA FINANCEIRA LTDA. (ATUAL CAPITAL ASSESSORIA E EMPREENDIMENTOS LTDA.)</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=2002&amp;NumProc=6</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>642</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>05.706.592/0001-85</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>BANCO BOZANO, SIMONSEN S/A</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=1999&amp;NumProc=10</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>00.659.559/0002-09</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>MASTER CORRETORA DE MERCADORIAS LTDA.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=IA&amp;Ano=2006&amp;NumProc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
         <v>4</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B37" t="inlineStr">
         <is>
           <t>00.016.087/6747-72</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>MARCOS LEVY</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>http://sistemas.cvm.gov.br/asp/cvmwww/inqueritos/DetPasAndamento.asp?sg_uf=RJ&amp;Ano=2006&amp;NumProc=8625</t>
         </is>

</xml_diff>